<commit_message>
Added function to calculate prevalence with time-varying ascertainment rates
</commit_message>
<xml_diff>
--- a/pars/limitations_table.xlsx
+++ b/pars/limitations_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/GitHub/covback/pars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34F3AFF2-53C4-1444-92ED-1083B0EB5169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBACFE86-FA78-CB48-99F8-13E82C2E7D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1300" windowWidth="51200" windowHeight="28340" xr2:uid="{EEF93CA8-125B-504C-ACD7-10EE48DFEF71}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{EEF93CA8-125B-504C-ACD7-10EE48DFEF71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Parameter</t>
   </si>
@@ -92,15 +92,6 @@
     <t>Top 16 locations ranked by total flight volume from China, plus four additional locations to represent all inhabited continents</t>
   </si>
   <si>
-    <t>Force of exportation (FOE)</t>
-  </si>
-  <si>
-    <t>Callibration of FOE to numbers of imported cases</t>
-  </si>
-  <si>
-    <t>Assumes that the conversion from FOE to numbers holds for non-Wuhan Chinese cities is the same as for Wuhan</t>
-  </si>
-  <si>
     <t>Delay distributions used for back-calculation</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>The entire population of a city represents the pool of eligible travellers</t>
   </si>
   <si>
-    <t>Conversion from FOE to actual numbers is based on detected imported cases in high surveillance locations from Wuhan</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -249,9 +237,6 @@
   </si>
   <si>
     <t>Assumed 5 million travelers between 10 and 25 January following assumptions made by Sanche et al.</t>
-  </si>
-  <si>
-    <t>There are no additional data available to test this claim, as cases imported from non-Wuhan Chinese cities were not reported</t>
   </si>
 </sst>
 </file>
@@ -657,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B11A67-C40A-9D46-8C21-EF9FAE1EB59A}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="49.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.2">
@@ -699,16 +684,16 @@
         <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.2">
@@ -722,13 +707,13 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
@@ -736,19 +721,19 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.2">
@@ -756,19 +741,19 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.2">
@@ -779,16 +764,16 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.2">
@@ -796,19 +781,19 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.2">
@@ -819,16 +804,16 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.2">
@@ -845,10 +830,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.2">
@@ -859,16 +844,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.2">
@@ -876,19 +861,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -896,19 +881,19 @@
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.2">
@@ -919,16 +904,16 @@
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.2">
@@ -936,39 +921,19 @@
         <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>